<commit_message>
*cambios en archivo plantilla de atenciones médicas
</commit_message>
<xml_diff>
--- a/public/files/templates/ANEXO4_8.xlsx
+++ b/public/files/templates/ANEXO4_8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krlit\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBD7358-08FA-4839-A749-7AAB9EC19936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476CD959-9831-43FA-9CFF-E95C1DE271AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{632ED216-0536-4FFC-B283-C552CE5EE223}"/>
   </bookViews>
@@ -345,7 +345,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>Estado</t>
   </si>
@@ -485,42 +485,6 @@
     <t>FECHA ULTIMO ELECTROCARDIOGRAMA</t>
   </si>
   <si>
-    <t>Fecha Control Enero</t>
-  </si>
-  <si>
-    <t>Fecha Control Febrero</t>
-  </si>
-  <si>
-    <t>Fecha Control Marzo</t>
-  </si>
-  <si>
-    <t>Fecha Control Abril</t>
-  </si>
-  <si>
-    <t>Fecha Control Mayo</t>
-  </si>
-  <si>
-    <t>Fecha Control Junio</t>
-  </si>
-  <si>
-    <t>Fecha Control Julio</t>
-  </si>
-  <si>
-    <t>Fecha Control Agosto</t>
-  </si>
-  <si>
-    <t>Fecha Control Septiembre</t>
-  </si>
-  <si>
-    <t>Fecha Control Octubre</t>
-  </si>
-  <si>
-    <t>Fecha Control Noviembre</t>
-  </si>
-  <si>
-    <t>Fecha Control Diciembre</t>
-  </si>
-  <si>
     <t>Recibio Medicamentos</t>
   </si>
   <si>
@@ -690,78 +654,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Estadio ER</t>
-  </si>
-  <si>
-    <t>TAS Enero</t>
-  </si>
-  <si>
-    <t>TAD Enero</t>
-  </si>
-  <si>
-    <t>TAS Febrero</t>
-  </si>
-  <si>
-    <t>TAD Febrero</t>
-  </si>
-  <si>
-    <t>TAS Marzo</t>
-  </si>
-  <si>
-    <t>TAD Marzo</t>
-  </si>
-  <si>
-    <t>TAS Abril</t>
-  </si>
-  <si>
-    <t>TAD Abril</t>
-  </si>
-  <si>
-    <t>TAS Mayo</t>
-  </si>
-  <si>
-    <t>TAD Mayo</t>
-  </si>
-  <si>
-    <t>TAS Junio</t>
-  </si>
-  <si>
-    <t>TAD Junio</t>
-  </si>
-  <si>
-    <t>TAS Julio</t>
-  </si>
-  <si>
-    <t>TAD Julio</t>
-  </si>
-  <si>
-    <t>TAS Agosto</t>
-  </si>
-  <si>
-    <t>TAD Agosto</t>
-  </si>
-  <si>
-    <t>TAS Septiembre</t>
-  </si>
-  <si>
-    <t>TAD Septiembre</t>
-  </si>
-  <si>
-    <t>TAS Octubre</t>
-  </si>
-  <si>
-    <t>TAD Octubre</t>
-  </si>
-  <si>
-    <t>TAS Noviembre</t>
-  </si>
-  <si>
-    <t>TAD Noviembre</t>
-  </si>
-  <si>
-    <t>TAS Diciembre</t>
-  </si>
-  <si>
-    <t>TAD Diciembre</t>
   </si>
 </sst>
 </file>
@@ -1398,10 +1290,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD6AD39-09F9-4CC9-ACF5-6F2F78A49C8B}">
-  <dimension ref="A1:EI100"/>
+  <dimension ref="A1:CY100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="AT11" sqref="AT11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,33 +1304,33 @@
     <col min="32" max="32" width="10.85546875" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:139" ht="120" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:103" ht="119.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>1</v>
@@ -1447,10 +1339,10 @@
         <v>2</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>3</v>
@@ -1465,43 +1357,43 @@
         <v>6</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="V1" s="36" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="X1" s="36" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Y1" s="8" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="AA1" s="8" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="AB1" s="8" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="AC1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="AD1" s="10" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="AE1" s="11" t="s">
         <v>10</v>
@@ -1519,7 +1411,7 @@
         <v>14</v>
       </c>
       <c r="AJ1" s="12" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>15</v>
@@ -1534,25 +1426,25 @@
         <v>18</v>
       </c>
       <c r="AO1" s="13" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="AP1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="AQ1" s="6" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="AR1" s="6" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="AS1" s="14" t="s">
         <v>20</v>
       </c>
       <c r="AT1" s="15" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="AU1" s="16" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="AV1" s="15" t="s">
         <v>21</v>
@@ -1609,10 +1501,10 @@
         <v>38</v>
       </c>
       <c r="BN1" s="21" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="BO1" s="21" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="BP1" s="16" t="s">
         <v>39</v>
@@ -1621,37 +1513,37 @@
         <v>40</v>
       </c>
       <c r="BR1" s="16" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="BS1" s="22" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="BT1" s="23" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="BU1" s="23" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="BV1" s="24" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="BW1" s="23" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="BX1" s="24" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="BY1" s="23" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="BZ1" s="24" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="CA1" s="23" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="CB1" s="24" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="CC1" s="25" t="s">
         <v>41</v>
@@ -1660,178 +1552,70 @@
         <v>42</v>
       </c>
       <c r="CE1" s="6" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="CF1" s="6" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="CG1" s="25" t="s">
         <v>43</v>
       </c>
       <c r="CH1" s="25" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="CI1" s="26" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="CJ1" s="27" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="CK1" s="27" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="CL1" s="28" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="CM1" s="4" t="s">
         <v>44</v>
       </c>
       <c r="CN1" s="4" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="CO1" s="4" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="CP1" s="4" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="CQ1" s="4" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="CR1" s="4" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="CS1" s="29" t="s">
         <v>45</v>
       </c>
       <c r="CT1" s="30" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="CU1" s="30" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="CV1" s="31" t="s">
         <v>46</v>
       </c>
       <c r="CW1" s="31" t="s">
-        <v>115</v>
+        <v>47</v>
       </c>
       <c r="CX1" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="CY1" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="CZ1" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="DA1" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="DB1" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="DC1" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="DD1" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="DE1" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="DF1" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="DG1" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="DH1" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="DI1" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="DJ1" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="DK1" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="DL1" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="DM1" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="DN1" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="DO1" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="DP1" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="DQ1" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="DR1" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="DS1" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="DT1" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="DU1" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="DV1" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="DW1" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="DX1" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="DY1" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="DZ1" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="EA1" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="EB1" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="EC1" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="ED1" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="EE1" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="EF1" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="EG1" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="EH1" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="EI1" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:139" x14ac:dyDescent="0.25">
+      <c r="CY1" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:103" x14ac:dyDescent="0.25">
       <c r="T2" s="32"/>
       <c r="U2" s="33"/>
       <c r="AA2" s="34"/>
@@ -1845,7 +1629,7 @@
       <c r="BG2" s="34"/>
       <c r="BI2" s="34"/>
     </row>
-    <row r="3" spans="1:139" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.25">
       <c r="T3" s="32"/>
       <c r="U3" s="33"/>
       <c r="AA3" s="34"/>
@@ -1858,7 +1642,7 @@
       <c r="BG3" s="34"/>
       <c r="BI3" s="34"/>
     </row>
-    <row r="4" spans="1:139" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:103" x14ac:dyDescent="0.25">
       <c r="T4" s="32"/>
       <c r="U4" s="33"/>
       <c r="AA4" s="34"/>
@@ -1871,7 +1655,7 @@
       <c r="BG4" s="34"/>
       <c r="BI4" s="34"/>
     </row>
-    <row r="5" spans="1:139" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:103" x14ac:dyDescent="0.25">
       <c r="T5" s="32"/>
       <c r="U5" s="33"/>
       <c r="AA5" s="34"/>
@@ -1884,7 +1668,7 @@
       <c r="BG5" s="34"/>
       <c r="BI5" s="34"/>
     </row>
-    <row r="6" spans="1:139" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:103" x14ac:dyDescent="0.25">
       <c r="T6" s="32"/>
       <c r="U6" s="33"/>
       <c r="AA6" s="34"/>
@@ -1897,7 +1681,7 @@
       <c r="BG6" s="34"/>
       <c r="BI6" s="34"/>
     </row>
-    <row r="7" spans="1:139" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:103" x14ac:dyDescent="0.25">
       <c r="T7" s="32"/>
       <c r="U7" s="33"/>
       <c r="AA7" s="34"/>
@@ -1910,7 +1694,7 @@
       <c r="BG7" s="34"/>
       <c r="BI7" s="34"/>
     </row>
-    <row r="8" spans="1:139" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:103" x14ac:dyDescent="0.25">
       <c r="T8" s="32"/>
       <c r="U8" s="33"/>
       <c r="AA8" s="34"/>
@@ -1923,7 +1707,7 @@
       <c r="BG8" s="34"/>
       <c r="BI8" s="34"/>
     </row>
-    <row r="9" spans="1:139" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:103" x14ac:dyDescent="0.25">
       <c r="T9" s="32"/>
       <c r="U9" s="33"/>
       <c r="AA9" s="34"/>
@@ -1936,7 +1720,7 @@
       <c r="BG9" s="34"/>
       <c r="BI9" s="34"/>
     </row>
-    <row r="10" spans="1:139" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:103" x14ac:dyDescent="0.25">
       <c r="T10" s="32"/>
       <c r="U10" s="33"/>
       <c r="AA10" s="34"/>
@@ -1949,7 +1733,7 @@
       <c r="BG10" s="34"/>
       <c r="BI10" s="34"/>
     </row>
-    <row r="11" spans="1:139" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:103" x14ac:dyDescent="0.25">
       <c r="T11" s="32"/>
       <c r="U11" s="33"/>
       <c r="AA11" s="34"/>
@@ -1962,7 +1746,7 @@
       <c r="BG11" s="34"/>
       <c r="BI11" s="34"/>
     </row>
-    <row r="12" spans="1:139" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:103" x14ac:dyDescent="0.25">
       <c r="T12" s="32"/>
       <c r="U12" s="33"/>
       <c r="AA12" s="34"/>
@@ -1975,7 +1759,7 @@
       <c r="BG12" s="34"/>
       <c r="BI12" s="34"/>
     </row>
-    <row r="13" spans="1:139" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:103" x14ac:dyDescent="0.25">
       <c r="T13" s="32"/>
       <c r="U13" s="33"/>
       <c r="AA13" s="34"/>
@@ -1988,7 +1772,7 @@
       <c r="BG13" s="34"/>
       <c r="BI13" s="34"/>
     </row>
-    <row r="14" spans="1:139" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:103" x14ac:dyDescent="0.25">
       <c r="T14" s="32"/>
       <c r="U14" s="33"/>
       <c r="AA14" s="34"/>
@@ -2001,7 +1785,7 @@
       <c r="BG14" s="34"/>
       <c r="BI14" s="34"/>
     </row>
-    <row r="15" spans="1:139" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:103" x14ac:dyDescent="0.25">
       <c r="T15" s="32"/>
       <c r="U15" s="33"/>
       <c r="AA15" s="34"/>
@@ -2014,7 +1798,7 @@
       <c r="BG15" s="34"/>
       <c r="BI15" s="34"/>
     </row>
-    <row r="16" spans="1:139" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:103" x14ac:dyDescent="0.25">
       <c r="T16" s="32"/>
       <c r="U16" s="33"/>
       <c r="AA16" s="34"/>

</xml_diff>